<commit_message>
Fixes datetime picker format, modal background issue, and destroys picker when necessary
</commit_message>
<xml_diff>
--- a/app/tables/eonasdan/forms/eonasdan/eonasdan.xlsx
+++ b/app/tables/eonasdan/forms/eonasdan/eonasdan.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="20115" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="5640" yWindow="2060" windowWidth="24000" windowHeight="12740"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>branch_label</t>
   </si>
@@ -53,12 +58,6 @@
     <t>templatePath</t>
   </si>
   <si>
-    <t>inputAttributes.min</t>
-  </si>
-  <si>
-    <t>inputAttributes.max</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
@@ -83,9 +82,6 @@
     <t>Date and Time</t>
   </si>
   <si>
-    <t>inputAttributes.data-field</t>
-  </si>
-  <si>
     <t>setting_name</t>
   </si>
   <si>
@@ -111,13 +107,40 @@
   </si>
   <si>
     <t>showFooter</t>
+  </si>
+  <si>
+    <t>example2</t>
+  </si>
+  <si>
+    <t>example3</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>inputAttributes.timeFormat</t>
+  </si>
+  <si>
+    <t>YYYY/DD/MM</t>
+  </si>
+  <si>
+    <t>HH:mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +179,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,13 +213,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -199,7 +240,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 2 2" xfId="4"/>
@@ -504,28 +547,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -564,7 +605,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>12</v>
@@ -575,32 +616,60 @@
       <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -608,67 +677,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="B3" s="5">
         <v>20141120</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>1</v>
@@ -677,6 +746,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>